<commit_message>
Projetos Aula01 solucao ex4
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -106,7 +106,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,14 +117,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,11 +146,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +466,7 @@
       <c r="B2" s="2">
         <v>44200</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>44201</v>
       </c>
       <c r="D2" s="2">
@@ -695,7 +687,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +696,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -724,50 +716,79 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
         <v>10</v>
       </c>
     </row>
@@ -775,40 +796,64 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B14" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B15" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Projetos aula02 Lista Mega
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="FREQ" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="25">
   <si>
     <t>NOME</t>
   </si>
@@ -433,9 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -489,6 +487,9 @@
       <c r="C3" t="s">
         <v>22</v>
       </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -500,6 +501,9 @@
       <c r="C4" t="s">
         <v>22</v>
       </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -511,6 +515,9 @@
       <c r="C5" t="s">
         <v>22</v>
       </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -522,6 +529,9 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -533,6 +543,9 @@
       <c r="C7" t="s">
         <v>22</v>
       </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -544,6 +557,9 @@
       <c r="C8" t="s">
         <v>23</v>
       </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -555,6 +571,9 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -566,6 +585,9 @@
       <c r="C10" t="s">
         <v>22</v>
       </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -577,6 +599,9 @@
       <c r="C11" t="s">
         <v>22</v>
       </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -587,6 +612,9 @@
       </c>
       <c r="C12" t="s">
         <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -599,6 +627,9 @@
       <c r="C13" t="s">
         <v>22</v>
       </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -610,6 +641,9 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -621,6 +655,9 @@
       <c r="C15" t="s">
         <v>22</v>
       </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -632,8 +669,11 @@
       <c r="C16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -643,8 +683,11 @@
       <c r="C17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -654,8 +697,11 @@
       <c r="C18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -665,8 +711,11 @@
       <c r="C19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -674,6 +723,9 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -686,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Chamada 3DES de 08-01-2021
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="25">
   <si>
     <t>NOME</t>
   </si>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +442,7 @@
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -458,8 +458,23 @@
       <c r="F1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,8 +493,23 @@
       <c r="F2" s="2">
         <v>44204</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2">
+        <v>44207</v>
+      </c>
+      <c r="H2" s="2">
+        <v>44208</v>
+      </c>
+      <c r="I2" s="2">
+        <v>44209</v>
+      </c>
+      <c r="J2" s="2">
+        <v>44210</v>
+      </c>
+      <c r="K2" s="2">
+        <v>44211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -495,8 +525,11 @@
       <c r="E3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -512,8 +545,11 @@
       <c r="E4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -529,8 +565,11 @@
       <c r="E5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -546,8 +585,11 @@
       <c r="E6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -563,8 +605,11 @@
       <c r="E7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -580,8 +625,11 @@
       <c r="E8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -597,8 +645,11 @@
       <c r="E9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -614,8 +665,11 @@
       <c r="E10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -631,8 +685,11 @@
       <c r="E11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -648,8 +705,11 @@
       <c r="E12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -665,8 +725,11 @@
       <c r="E13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -682,8 +745,11 @@
       <c r="E14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -699,8 +765,11 @@
       <c r="E15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -716,8 +785,11 @@
       <c r="E16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -733,8 +805,11 @@
       <c r="E17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -750,8 +825,11 @@
       <c r="E18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -767,8 +845,11 @@
       <c r="E19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -782,6 +863,9 @@
         <v>22</v>
       </c>
       <c r="E20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
3DES Adicionada aula 1 RMS
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\senai2021\3des\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2021\3des\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="25">
   <si>
     <t>NOME</t>
   </si>
@@ -433,9 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -528,6 +526,9 @@
       <c r="F3" t="s">
         <v>22</v>
       </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -548,6 +549,9 @@
       <c r="F4" t="s">
         <v>22</v>
       </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -568,6 +572,9 @@
       <c r="F5" t="s">
         <v>22</v>
       </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -588,6 +595,9 @@
       <c r="F6" t="s">
         <v>22</v>
       </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -608,6 +618,9 @@
       <c r="F7" t="s">
         <v>23</v>
       </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -628,6 +641,9 @@
       <c r="F8" t="s">
         <v>23</v>
       </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -648,6 +664,9 @@
       <c r="F9" t="s">
         <v>23</v>
       </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -668,6 +687,9 @@
       <c r="F10" t="s">
         <v>23</v>
       </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -688,6 +710,9 @@
       <c r="F11" t="s">
         <v>22</v>
       </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -707,6 +732,9 @@
       </c>
       <c r="F12" t="s">
         <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -728,6 +756,9 @@
       <c r="F13" t="s">
         <v>22</v>
       </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -748,6 +779,9 @@
       <c r="F14" t="s">
         <v>22</v>
       </c>
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -768,6 +802,9 @@
       <c r="F15" t="s">
         <v>22</v>
       </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -788,8 +825,11 @@
       <c r="F16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -808,8 +848,11 @@
       <c r="F17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -828,8 +871,11 @@
       <c r="F18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -848,8 +894,11 @@
       <c r="F19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -866,6 +915,9 @@
         <v>22</v>
       </c>
       <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
3DES Projetos aula02 solucao exercicios sena
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FREQ" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="26">
   <si>
     <t>NOME</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
   </si>
 </sst>
 </file>
@@ -433,7 +436,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -529,6 +534,9 @@
       <c r="G3" t="s">
         <v>22</v>
       </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -552,6 +560,9 @@
       <c r="G4" t="s">
         <v>22</v>
       </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -575,6 +586,9 @@
       <c r="G5" t="s">
         <v>22</v>
       </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -598,6 +612,9 @@
       <c r="G6" t="s">
         <v>22</v>
       </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -621,6 +638,9 @@
       <c r="G7" t="s">
         <v>23</v>
       </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -644,6 +664,9 @@
       <c r="G8" t="s">
         <v>22</v>
       </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -667,6 +690,9 @@
       <c r="G9" t="s">
         <v>22</v>
       </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -690,6 +716,9 @@
       <c r="G10" t="s">
         <v>23</v>
       </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -713,6 +742,9 @@
       <c r="G11" t="s">
         <v>22</v>
       </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -735,6 +767,9 @@
       </c>
       <c r="G12" t="s">
         <v>23</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -759,6 +794,9 @@
       <c r="G13" t="s">
         <v>22</v>
       </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -782,6 +820,9 @@
       <c r="G14" t="s">
         <v>22</v>
       </c>
+      <c r="H14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -805,6 +846,9 @@
       <c r="G15" t="s">
         <v>23</v>
       </c>
+      <c r="H15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -828,8 +872,11 @@
       <c r="G16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -851,8 +898,11 @@
       <c r="G17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -874,8 +924,11 @@
       <c r="G18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -897,8 +950,11 @@
       <c r="G19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -918,6 +974,9 @@
         <v>22</v>
       </c>
       <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -930,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,6 +1002,9 @@
       <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -951,7 +1013,9 @@
       <c r="B2" s="2">
         <v>44201</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2">
+        <v>44208</v>
+      </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -963,6 +1027,9 @@
       <c r="B3" s="5">
         <v>10</v>
       </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -971,6 +1038,9 @@
       <c r="B4">
         <v>10</v>
       </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -979,6 +1049,9 @@
       <c r="B5">
         <v>5</v>
       </c>
+      <c r="C5">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -987,6 +1060,9 @@
       <c r="B6">
         <v>10</v>
       </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -995,6 +1071,9 @@
       <c r="B7">
         <v>10</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1003,6 +1082,9 @@
       <c r="B8">
         <v>0</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1011,6 +1093,9 @@
       <c r="B9">
         <v>0</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1019,6 +1104,9 @@
       <c r="B10">
         <v>10</v>
       </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1027,6 +1115,9 @@
       <c r="B11">
         <v>10</v>
       </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1034,6 +1125,9 @@
       </c>
       <c r="B12">
         <v>10</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1043,6 +1137,9 @@
       <c r="B13">
         <v>10</v>
       </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1051,6 +1148,9 @@
       <c r="B14" s="5">
         <v>10</v>
       </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1059,6 +1159,9 @@
       <c r="B15" s="5">
         <v>10</v>
       </c>
+      <c r="C15">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1067,37 +1170,52 @@
       <c r="B16">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20">
         <v>10</v>
+      </c>
+      <c r="C20">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1DES FPOO anexado link exemplo SORT
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="27">
   <si>
     <t>NOME</t>
   </si>
@@ -440,7 +440,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +546,9 @@
       <c r="J3" t="s">
         <v>22</v>
       </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -576,6 +579,9 @@
         <v>22</v>
       </c>
       <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -610,6 +616,9 @@
       <c r="J5" t="s">
         <v>23</v>
       </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -642,6 +651,9 @@
       <c r="J6" t="s">
         <v>22</v>
       </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -674,6 +686,9 @@
       <c r="J7" t="s">
         <v>23</v>
       </c>
+      <c r="K7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -706,6 +721,9 @@
       <c r="J8" t="s">
         <v>23</v>
       </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -738,6 +756,9 @@
       <c r="J9" t="s">
         <v>22</v>
       </c>
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -770,6 +791,9 @@
       <c r="J10" t="s">
         <v>23</v>
       </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -802,6 +826,9 @@
       <c r="J11" t="s">
         <v>22</v>
       </c>
+      <c r="K11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -834,6 +861,9 @@
       <c r="J12" t="s">
         <v>23</v>
       </c>
+      <c r="K12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -866,6 +896,9 @@
       <c r="J13" t="s">
         <v>22</v>
       </c>
+      <c r="K13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -898,6 +931,9 @@
       <c r="J14" t="s">
         <v>22</v>
       </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -930,6 +966,9 @@
       <c r="J15" t="s">
         <v>22</v>
       </c>
+      <c r="K15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -962,8 +1001,11 @@
       <c r="J16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -994,8 +1036,11 @@
       <c r="J17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1026,8 +1071,11 @@
       <c r="J18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1058,8 +1106,11 @@
       <c r="J19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1088,6 +1139,9 @@
         <v>22</v>
       </c>
       <c r="J20" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
3DES projetos aula06 Qualidade
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\senai2021\3des\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2021\3des\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FREQ" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,7 +1201,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1215,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1243,7 +1243,7 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1285,7 +1285,7 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1299,7 +1299,7 @@
         <v>2</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1327,7 +1327,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
         <v>4</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1355,7 +1355,7 @@
         <v>2</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
         <v>3</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1411,7 +1411,7 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1425,7 +1425,7 @@
         <v>4</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1439,7 +1439,7 @@
         <v>0.5</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3DES projetos - Adicionadas aulas de 06 a 10
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="FREQ" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="27">
   <si>
     <t>NOME</t>
   </si>
@@ -437,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +448,7 @@
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -479,8 +479,23 @@
       <c r="K1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,8 +529,23 @@
       <c r="K2" s="2">
         <v>44211</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="2">
+        <v>44214</v>
+      </c>
+      <c r="M2" s="2">
+        <v>44215</v>
+      </c>
+      <c r="N2" s="2">
+        <v>44216</v>
+      </c>
+      <c r="O2" s="2">
+        <v>44217</v>
+      </c>
+      <c r="P2" s="2">
+        <v>44218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -549,8 +579,14 @@
       <c r="K3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -584,8 +620,14 @@
       <c r="K4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -619,8 +661,14 @@
       <c r="K5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -654,8 +702,14 @@
       <c r="K6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -689,8 +743,14 @@
       <c r="K7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -724,8 +784,14 @@
       <c r="K8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -759,8 +825,14 @@
       <c r="K9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -794,8 +866,14 @@
       <c r="K10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -829,8 +907,14 @@
       <c r="K11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -864,8 +948,14 @@
       <c r="K12" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -899,8 +989,14 @@
       <c r="K13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -934,8 +1030,14 @@
       <c r="K14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -969,8 +1071,14 @@
       <c r="K15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1004,8 +1112,14 @@
       <c r="K16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1039,8 +1153,14 @@
       <c r="K17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1074,8 +1194,14 @@
       <c r="K18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1109,8 +1235,14 @@
       <c r="K19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1142,6 +1274,12 @@
         <v>22</v>
       </c>
       <c r="K20" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1154,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
3DES projetos aula07 Metodologias
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="FREQ" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="27">
   <si>
     <t>NOME</t>
   </si>
@@ -440,12 +440,13 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -585,6 +586,9 @@
       <c r="M3" t="s">
         <v>22</v>
       </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -624,6 +628,9 @@
         <v>22</v>
       </c>
       <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -667,6 +674,9 @@
       <c r="M5" t="s">
         <v>22</v>
       </c>
+      <c r="N5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -708,6 +718,9 @@
       <c r="M6" t="s">
         <v>22</v>
       </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -749,6 +762,9 @@
       <c r="M7" t="s">
         <v>23</v>
       </c>
+      <c r="N7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -790,6 +806,9 @@
       <c r="M8" t="s">
         <v>22</v>
       </c>
+      <c r="N8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -831,6 +850,9 @@
       <c r="M9" t="s">
         <v>22</v>
       </c>
+      <c r="N9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -872,6 +894,9 @@
       <c r="M10" t="s">
         <v>22</v>
       </c>
+      <c r="N10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -913,6 +938,9 @@
       <c r="M11" t="s">
         <v>22</v>
       </c>
+      <c r="N11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -954,6 +982,9 @@
       <c r="M12" t="s">
         <v>22</v>
       </c>
+      <c r="N12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -995,6 +1026,9 @@
       <c r="M13" t="s">
         <v>22</v>
       </c>
+      <c r="N13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1036,6 +1070,9 @@
       <c r="M14" t="s">
         <v>22</v>
       </c>
+      <c r="N14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1077,6 +1114,9 @@
       <c r="M15" t="s">
         <v>22</v>
       </c>
+      <c r="N15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1118,8 +1158,11 @@
       <c r="M16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1159,8 +1202,11 @@
       <c r="M17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1200,8 +1246,11 @@
       <c r="M18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1241,8 +1290,11 @@
       <c r="M19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1280,6 +1332,9 @@
         <v>22</v>
       </c>
       <c r="M20" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1293,7 +1348,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,10 +1472,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D9">
         <v>2</v>

</xml_diff>

<commit_message>
3DES projetos atualizada a estrutura de pastas
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="FREQ" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="28">
   <si>
     <t>NOME</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>L3-TAP</t>
+  </si>
+  <si>
+    <t>AT1-Cont</t>
   </si>
 </sst>
 </file>
@@ -439,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,6 +592,9 @@
       <c r="N3" t="s">
         <v>22</v>
       </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -631,6 +637,9 @@
         <v>22</v>
       </c>
       <c r="N4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -677,6 +686,9 @@
       <c r="N5" t="s">
         <v>22</v>
       </c>
+      <c r="O5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -721,6 +733,9 @@
       <c r="N6" t="s">
         <v>22</v>
       </c>
+      <c r="O6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -765,6 +780,9 @@
       <c r="N7" t="s">
         <v>22</v>
       </c>
+      <c r="O7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -809,6 +827,9 @@
       <c r="N8" t="s">
         <v>22</v>
       </c>
+      <c r="O8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -853,6 +874,9 @@
       <c r="N9" t="s">
         <v>22</v>
       </c>
+      <c r="O9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -897,6 +921,9 @@
       <c r="N10" t="s">
         <v>22</v>
       </c>
+      <c r="O10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -941,6 +968,9 @@
       <c r="N11" t="s">
         <v>22</v>
       </c>
+      <c r="O11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -985,6 +1015,9 @@
       <c r="N12" t="s">
         <v>22</v>
       </c>
+      <c r="O12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1029,6 +1062,9 @@
       <c r="N13" t="s">
         <v>22</v>
       </c>
+      <c r="O13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1073,6 +1109,9 @@
       <c r="N14" t="s">
         <v>22</v>
       </c>
+      <c r="O14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1117,6 +1156,9 @@
       <c r="N15" t="s">
         <v>22</v>
       </c>
+      <c r="O15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1161,8 +1203,11 @@
       <c r="N16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1205,8 +1250,11 @@
       <c r="N17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1249,8 +1297,11 @@
       <c r="N18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1293,8 +1344,11 @@
       <c r="N19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1335,6 +1389,9 @@
         <v>22</v>
       </c>
       <c r="N20" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1347,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,6 +1423,9 @@
       <c r="D1" t="s">
         <v>26</v>
       </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
3DES Projetos - Adicionada aula08 - Desavio
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="28">
   <si>
     <t>NOME</t>
   </si>
@@ -109,12 +109,6 @@
   </si>
   <si>
     <t>AT1-Cont</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>f</t>
   </si>
 </sst>
 </file>
@@ -446,19 +440,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="21" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -504,8 +501,23 @@
       <c r="P1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,8 +566,23 @@
       <c r="P2" s="2">
         <v>44218</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="2">
+        <v>44221</v>
+      </c>
+      <c r="R2" s="2">
+        <v>44222</v>
+      </c>
+      <c r="S2" s="2">
+        <v>44223</v>
+      </c>
+      <c r="T2" s="2">
+        <v>44224</v>
+      </c>
+      <c r="U2" s="2">
+        <v>44225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -602,10 +629,13 @@
         <v>22</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -652,10 +682,13 @@
         <v>22</v>
       </c>
       <c r="P4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -702,10 +735,13 @@
         <v>22</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -752,10 +788,13 @@
         <v>22</v>
       </c>
       <c r="P6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -802,10 +841,13 @@
         <v>23</v>
       </c>
       <c r="P7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -852,10 +894,13 @@
         <v>23</v>
       </c>
       <c r="P8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -902,10 +947,13 @@
         <v>22</v>
       </c>
       <c r="P9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -952,10 +1000,13 @@
         <v>22</v>
       </c>
       <c r="P10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1002,10 +1053,13 @@
         <v>22</v>
       </c>
       <c r="P11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1052,10 +1106,13 @@
         <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1102,10 +1159,13 @@
         <v>22</v>
       </c>
       <c r="P13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1152,10 +1212,13 @@
         <v>22</v>
       </c>
       <c r="P14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1202,10 +1265,13 @@
         <v>22</v>
       </c>
       <c r="P15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1252,10 +1318,13 @@
         <v>22</v>
       </c>
       <c r="P16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1302,10 +1371,13 @@
         <v>22</v>
       </c>
       <c r="P17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1352,10 +1424,13 @@
         <v>22</v>
       </c>
       <c r="P18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1402,10 +1477,13 @@
         <v>22</v>
       </c>
       <c r="P19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1452,7 +1530,10 @@
         <v>22</v>
       </c>
       <c r="P20" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3DES projetos Adicionada aula 11 Dados do pré-projeto
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="28">
   <si>
     <t>NOME</t>
   </si>
@@ -446,7 +446,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,6 +634,9 @@
       <c r="Q3" t="s">
         <v>23</v>
       </c>
+      <c r="R3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -685,6 +688,9 @@
         <v>22</v>
       </c>
       <c r="Q4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -740,6 +746,9 @@
       <c r="Q5" t="s">
         <v>22</v>
       </c>
+      <c r="R5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -793,6 +802,9 @@
       <c r="Q6" t="s">
         <v>22</v>
       </c>
+      <c r="R6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -846,6 +858,9 @@
       <c r="Q7" t="s">
         <v>23</v>
       </c>
+      <c r="R7" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -899,6 +914,9 @@
       <c r="Q8" t="s">
         <v>22</v>
       </c>
+      <c r="R8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -952,6 +970,9 @@
       <c r="Q9" t="s">
         <v>22</v>
       </c>
+      <c r="R9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1005,6 +1026,9 @@
       <c r="Q10" t="s">
         <v>22</v>
       </c>
+      <c r="R10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1058,6 +1082,9 @@
       <c r="Q11" t="s">
         <v>23</v>
       </c>
+      <c r="R11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -1111,6 +1138,9 @@
       <c r="Q12" t="s">
         <v>22</v>
       </c>
+      <c r="R12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1164,6 +1194,9 @@
       <c r="Q13" t="s">
         <v>23</v>
       </c>
+      <c r="R13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1217,6 +1250,9 @@
       <c r="Q14" t="s">
         <v>22</v>
       </c>
+      <c r="R14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1270,6 +1306,9 @@
       <c r="Q15" t="s">
         <v>22</v>
       </c>
+      <c r="R15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -1323,8 +1362,11 @@
       <c r="Q16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1376,8 +1418,11 @@
       <c r="Q17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1429,8 +1474,11 @@
       <c r="Q18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1482,8 +1530,11 @@
       <c r="Q19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1534,6 +1585,9 @@
       </c>
       <c r="Q20" t="s">
         <v>22</v>
+      </c>
+      <c r="R20" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1546,7 +1600,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1634,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
3DES projetos aula11 Divisao Missoes Grupos
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="28">
   <si>
     <t>NOME</t>
   </si>
@@ -446,7 +446,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T14" sqref="T14"/>
+      <selection pane="bottomRight" activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,7 +640,10 @@
       <c r="S3" t="s">
         <v>22</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -702,7 +705,10 @@
       <c r="S4" t="s">
         <v>22</v>
       </c>
-      <c r="T4" t="s">
+      <c r="T4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -764,8 +770,11 @@
       <c r="S5" t="s">
         <v>22</v>
       </c>
-      <c r="T5" t="s">
-        <v>22</v>
+      <c r="T5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -826,7 +835,10 @@
       <c r="S6" t="s">
         <v>22</v>
       </c>
-      <c r="T6" t="s">
+      <c r="T6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -888,7 +900,10 @@
       <c r="S7" t="s">
         <v>23</v>
       </c>
-      <c r="T7" t="s">
+      <c r="T7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -950,8 +965,11 @@
       <c r="S8" t="s">
         <v>22</v>
       </c>
-      <c r="T8" t="s">
-        <v>22</v>
+      <c r="T8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -1012,7 +1030,10 @@
       <c r="S9" t="s">
         <v>22</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1074,8 +1095,11 @@
       <c r="S10" t="s">
         <v>22</v>
       </c>
-      <c r="T10" t="s">
-        <v>23</v>
+      <c r="T10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1136,8 +1160,11 @@
       <c r="S11" t="s">
         <v>22</v>
       </c>
-      <c r="T11" t="s">
-        <v>23</v>
+      <c r="T11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -1198,7 +1225,10 @@
       <c r="S12" t="s">
         <v>22</v>
       </c>
-      <c r="T12" t="s">
+      <c r="T12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1260,7 +1290,10 @@
       <c r="S13" t="s">
         <v>22</v>
       </c>
-      <c r="T13" t="s">
+      <c r="T13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1322,8 +1355,11 @@
       <c r="S14" t="s">
         <v>22</v>
       </c>
-      <c r="T14" t="s">
-        <v>23</v>
+      <c r="T14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1384,7 +1420,10 @@
       <c r="S15" t="s">
         <v>22</v>
       </c>
-      <c r="T15" t="s">
+      <c r="T15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U15" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1446,11 +1485,14 @@
       <c r="S16" t="s">
         <v>22</v>
       </c>
-      <c r="T16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1508,11 +1550,14 @@
       <c r="S17" t="s">
         <v>22</v>
       </c>
-      <c r="T17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1570,11 +1615,14 @@
       <c r="S18" t="s">
         <v>22</v>
       </c>
-      <c r="T18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1632,11 +1680,14 @@
       <c r="S19" t="s">
         <v>22</v>
       </c>
-      <c r="T19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1694,12 +1745,16 @@
       <c r="S20" t="s">
         <v>22</v>
       </c>
-      <c r="T20" t="s">
-        <v>23</v>
+      <c r="T20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
3DES projetos aula11 atualizadas missoes
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="28">
   <si>
     <t>NOME</t>
   </si>
@@ -440,22 +440,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U9" sqref="U9"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="21" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="20" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -516,8 +517,23 @@
       <c r="U1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,8 +597,23 @@
       <c r="U2" s="2">
         <v>44225</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" s="2">
+        <v>44228</v>
+      </c>
+      <c r="W2" s="2">
+        <v>44229</v>
+      </c>
+      <c r="X2" s="2">
+        <v>44230</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>44231</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>44232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -646,8 +677,11 @@
       <c r="U3" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -711,8 +745,11 @@
       <c r="U4" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -776,8 +813,11 @@
       <c r="U5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -841,8 +881,11 @@
       <c r="U6" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -906,8 +949,11 @@
       <c r="U7" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -971,8 +1017,11 @@
       <c r="U8" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1036,8 +1085,11 @@
       <c r="U9" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1101,8 +1153,11 @@
       <c r="U10" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1166,8 +1221,11 @@
       <c r="U11" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1231,8 +1289,11 @@
       <c r="U12" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1296,8 +1357,11 @@
       <c r="U13" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1361,8 +1425,11 @@
       <c r="U14" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1426,8 +1493,11 @@
       <c r="U15" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1491,8 +1561,11 @@
       <c r="U16" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1556,8 +1629,11 @@
       <c r="U17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1621,8 +1697,11 @@
       <c r="U18" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1686,8 +1765,11 @@
       <c r="U19" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1750,6 +1832,9 @@
       </c>
       <c r="U20" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="V20" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aula do dia 26/03
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2021\3des\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\2021\Senai\Matérias\senai2021\3des\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B40902-CCF1-4C24-A899-E9923A91F1FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="9195"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FREQ" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="30">
   <si>
     <t>NOME</t>
   </si>
@@ -120,7 +121,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -445,24 +446,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AG20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA17" sqref="AA17"/>
+      <selection pane="bottomRight" activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="20" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="6.7109375" customWidth="1"/>
+    <col min="2" max="20" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -538,8 +539,29 @@
       <c r="Z1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,8 +640,19 @@
       <c r="Z2" s="2">
         <v>44232</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA2" s="2">
+        <v>44280</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>44281</v>
+      </c>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -689,8 +722,11 @@
       <c r="Z3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -760,8 +796,11 @@
       <c r="Z4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -832,7 +871,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -902,8 +941,11 @@
       <c r="Z6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -973,8 +1015,11 @@
       <c r="Z7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1044,8 +1089,11 @@
       <c r="Z8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1115,8 +1163,11 @@
       <c r="Z9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1186,8 +1237,11 @@
       <c r="Z10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1257,8 +1311,11 @@
       <c r="Z11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1328,8 +1385,11 @@
       <c r="Z12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1399,8 +1459,11 @@
       <c r="Z13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1470,8 +1533,11 @@
       <c r="Z14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1541,8 +1607,11 @@
       <c r="Z15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1612,8 +1681,11 @@
       <c r="Z16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1683,8 +1755,11 @@
       <c r="Z17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1754,8 +1829,11 @@
       <c r="Z18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1825,8 +1903,11 @@
       <c r="Z19" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1895,6 +1976,9 @@
       </c>
       <c r="Z20" t="s">
         <v>29</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1904,19 +1988,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>25</v>
       </c>
@@ -1930,7 +2014,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1948,7 +2032,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1965,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1982,7 +2066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1999,7 +2083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2016,7 +2100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2033,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2050,7 +2134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2067,7 +2151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2084,7 +2168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2101,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2118,7 +2202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2135,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2152,7 +2236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2169,7 +2253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2186,7 +2270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2203,7 +2287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2220,7 +2304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2237,7 +2321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
1des fpoo questionario final
</commit_message>
<xml_diff>
--- a/3des/3desfreq.xlsx
+++ b/3des/3desfreq.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SENAI\senai2021\3des\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wellington\senai2021\3des\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01AA980-5173-4718-B488-1CEA6D133B2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102F45F6-D8A6-4250-88D2-C24014387838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6810" yWindow="2685" windowWidth="13680" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FREQ" sheetId="1" r:id="rId1"/>
     <sheet name="PONTOS" sheetId="2" r:id="rId2"/>
+    <sheet name="AvaliaçãoProjetos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="82">
   <si>
     <t>NOME</t>
   </si>
@@ -116,13 +117,169 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>Natureza dos Critérios</t>
+  </si>
+  <si>
+    <t>Fundamentos Técnicos e Científicos ou Capacidades Técnicas</t>
+  </si>
+  <si>
+    <t>Critérios de avaliação</t>
+  </si>
+  <si>
+    <t>Crítico</t>
+  </si>
+  <si>
+    <t>Desejável</t>
+  </si>
+  <si>
+    <t>NÃO Atingiu</t>
+  </si>
+  <si>
+    <t>Atingiu</t>
+  </si>
+  <si>
+    <t>Formativa</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Somativa</t>
+  </si>
+  <si>
+    <t>Competências Técnicas</t>
+  </si>
+  <si>
+    <t>6. Definir o custo estimado para o desenvolvimento dos componentes</t>
+  </si>
+  <si>
+    <t>7. Definir os softwares a serem utilizados no desenvolvimento do sistema (2)</t>
+  </si>
+  <si>
+    <t>Manter coerência na escolha do ambiente e linguagem de programação demonstrando eficácia  (Deve solucionar o problema apresentado).</t>
+  </si>
+  <si>
+    <t>8. Definir as dependências de software considerando os componentes do sistema, para a sua im-plantação</t>
+  </si>
+  <si>
+    <t>5. Elaborar cronograma das etapas sequenciadas do desenvolvimento dos componentes, considerando a integração com outros profissionais envolvidos no projeto (2)</t>
+  </si>
+  <si>
+    <t>Representar as tarefas e executores utilizando a ferramenta gráfico de Gantt.</t>
+  </si>
+  <si>
+    <t>12. Pesquisar em diversas fontes de informação tendo em vista as melhores práticas de mercado considerando, inclusive, a performance e a qualidade de software (21)10. Implementar as funcionali-dades de acordo com os requisitos definidos</t>
+  </si>
+  <si>
+    <t>Representar a pesquisa utilizando a análise SWOT.</t>
+  </si>
+  <si>
+    <t>10. Implementar as funcionalidades de acordo com os requisitos definidos</t>
+  </si>
+  <si>
+    <t>11. Apresentar tecnicamente ao cliente o sistema de software desenvolvido, sanando as possíveis dúvidas sobre o funcionamento do mesmo</t>
+  </si>
+  <si>
+    <t>Manter postura profissional, demonstrar habilidades de comunicação e responder as questões demonstrando confiança.</t>
+  </si>
+  <si>
+    <t>Competências de Gestão</t>
+  </si>
+  <si>
+    <t>5. Demonstrar visão holística</t>
+  </si>
+  <si>
+    <t>Expressar qual é o problema através da documentação e demonstrar a solução implementada como um todo.</t>
+  </si>
+  <si>
+    <t>7. Manter relacionamento interpessoal</t>
+  </si>
+  <si>
+    <t>Demonstrar o que cada integrante do grupo realmente executou de forma profissional e imparcial.</t>
+  </si>
+  <si>
+    <t>9. Trabalhar em equipe (2)</t>
+  </si>
+  <si>
+    <t>10. Comunicar-se com clareza</t>
+  </si>
+  <si>
+    <t>Apresentar as ideias de forma completa, íntegra e completa.</t>
+  </si>
+  <si>
+    <t>Saber estimar o custo e tempo gasto, registrar via cronograma e responder a questionamentos durante a apresentação.</t>
+  </si>
+  <si>
+    <t>Fazer a gestão de dependências manualmente ou por framework evidenciar com o resultado das funcionalidades e conteúdos das interfaces de usuário</t>
+  </si>
+  <si>
+    <t>Cada funcionalidade proposta e documentada deve funcionar de maneira a cumprir o requisito proposto</t>
+  </si>
+  <si>
+    <t>Nível de Desempenho</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>NÍVEIS DE DESEMPENHO</t>
+  </si>
+  <si>
+    <t>NÍVEIS</t>
+  </si>
+  <si>
+    <t>NOTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atingiu todos os critérios críticos e desejáveis </t>
+  </si>
+  <si>
+    <t>Atingiu todos os critérios críticos e 5 desejáveis</t>
+  </si>
+  <si>
+    <t>Atingiu todos os critérios críticos e 4 desejáveis</t>
+  </si>
+  <si>
+    <t>Atingiu todos os critérios críticos e 3 desejáveis</t>
+  </si>
+  <si>
+    <t>Atingiu todos os critérios críticos e 2 desejáveis</t>
+  </si>
+  <si>
+    <t>Atingiu todos os critérios críticos e 1 desejáveis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atingiu todos os critérios críticos </t>
+  </si>
+  <si>
+    <t>Atingiu 4 critérios críticos</t>
+  </si>
+  <si>
+    <t>Atingiu 3 critérios críticos</t>
+  </si>
+  <si>
+    <t>Atingiu 2 critérios críticos</t>
+  </si>
+  <si>
+    <t>Atingiu 1 critério crítico</t>
+  </si>
+  <si>
+    <t>Transmitir harmonia do grupo durante a apresentação e em todas as entregas: - Documento do Projeto, Repositório com Códigos Fonte.</t>
+  </si>
+  <si>
+    <t>PreProjeto</t>
+  </si>
+  <si>
+    <t>ProjetoFinal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,16 +302,104 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4F81BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -162,11 +407,469 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -176,6 +879,165 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,11 +1320,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE23" sqref="AE23"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2057,18 +2919,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>25</v>
       </c>
@@ -2081,8 +2944,14 @@
       <c r="E1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2098,9 +2967,14 @@
       <c r="E2" s="2">
         <v>44221</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="2">
+        <v>44301</v>
+      </c>
+      <c r="G2" s="2">
+        <v>44384</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2117,7 +2991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -2134,7 +3008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2151,7 +3025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2168,7 +3042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2185,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2202,7 +3076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2219,7 +3093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2236,7 +3110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2253,7 +3127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2270,7 +3144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2287,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2304,7 +3178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2321,7 +3195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2410,4 +3284,719 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EEBC346-3D53-4B5C-9FF8-3DD902732840}">
+  <dimension ref="A1:X36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="55.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="7" max="24" width="3.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="121.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="U1" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="V1" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="W1" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" s="46" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="47"/>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="47"/>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="18"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="49"/>
+    </row>
+    <row r="5" spans="1:24" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
+      <c r="V5" s="38"/>
+      <c r="W5" s="38"/>
+      <c r="X5" s="39"/>
+    </row>
+    <row r="6" spans="1:24" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="36"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="41"/>
+    </row>
+    <row r="7" spans="1:24" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="36"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="36"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="36"/>
+      <c r="T7" s="36"/>
+      <c r="U7" s="36"/>
+      <c r="V7" s="36"/>
+      <c r="W7" s="36"/>
+      <c r="X7" s="41"/>
+    </row>
+    <row r="8" spans="1:24" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="36"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="36"/>
+      <c r="P8" s="36"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="36"/>
+      <c r="S8" s="36"/>
+      <c r="T8" s="36"/>
+      <c r="U8" s="36"/>
+      <c r="V8" s="36"/>
+      <c r="W8" s="36"/>
+      <c r="X8" s="41"/>
+    </row>
+    <row r="9" spans="1:24" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="36"/>
+      <c r="U9" s="36"/>
+      <c r="V9" s="36"/>
+      <c r="W9" s="36"/>
+      <c r="X9" s="41"/>
+    </row>
+    <row r="10" spans="1:24" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="36"/>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="36"/>
+      <c r="V10" s="36"/>
+      <c r="W10" s="36"/>
+      <c r="X10" s="41"/>
+    </row>
+    <row r="11" spans="1:24" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36"/>
+      <c r="S11" s="36"/>
+      <c r="T11" s="36"/>
+      <c r="U11" s="36"/>
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="41"/>
+    </row>
+    <row r="12" spans="1:24" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="36"/>
+      <c r="P12" s="36"/>
+      <c r="Q12" s="36"/>
+      <c r="R12" s="36"/>
+      <c r="S12" s="36"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="41"/>
+    </row>
+    <row r="13" spans="1:24" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="36"/>
+      <c r="X13" s="41"/>
+    </row>
+    <row r="14" spans="1:24" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="41"/>
+    </row>
+    <row r="15" spans="1:24" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="43"/>
+      <c r="U15" s="43"/>
+      <c r="V15" s="43"/>
+      <c r="W15" s="43"/>
+      <c r="X15" s="44"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="55" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="58">
+        <v>1</v>
+      </c>
+      <c r="D25" s="59">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="58">
+        <v>2</v>
+      </c>
+      <c r="D26" s="59">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="58">
+        <v>3</v>
+      </c>
+      <c r="D27" s="59">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="58">
+        <v>4</v>
+      </c>
+      <c r="D28" s="59">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="58">
+        <v>5</v>
+      </c>
+      <c r="D29" s="59">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="58">
+        <v>6</v>
+      </c>
+      <c r="D30" s="59">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="61">
+        <v>7</v>
+      </c>
+      <c r="D31" s="62">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="58">
+        <v>9</v>
+      </c>
+      <c r="D32" s="59">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="58">
+        <v>10</v>
+      </c>
+      <c r="D33" s="59">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="58">
+        <v>11</v>
+      </c>
+      <c r="D34" s="59">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="64">
+        <v>12</v>
+      </c>
+      <c r="D35" s="65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="S1:S4"/>
+    <mergeCell ref="T1:T4"/>
+    <mergeCell ref="U1:U4"/>
+    <mergeCell ref="V1:V4"/>
+    <mergeCell ref="W1:W4"/>
+    <mergeCell ref="X1:X4"/>
+    <mergeCell ref="M1:M4"/>
+    <mergeCell ref="N1:N4"/>
+    <mergeCell ref="O1:O4"/>
+    <mergeCell ref="P1:P4"/>
+    <mergeCell ref="Q1:Q4"/>
+    <mergeCell ref="R1:R4"/>
+    <mergeCell ref="G1:G4"/>
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="I1:I4"/>
+    <mergeCell ref="J1:J4"/>
+    <mergeCell ref="K1:K4"/>
+    <mergeCell ref="L1:L4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="A5:A11"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>